<commit_message>
Improved Tasks 1 and 2 Backend
</commit_message>
<xml_diff>
--- a/back-end/Back-end Services.xlsx
+++ b/back-end/Back-end Services.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guicu\Documents\Universidade\Mestrado\2Semestre\Aplicações na web\aw-project\back-end\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C9B3D0-8265-4563-92E9-39D5E8C46268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05EB8880-0518-412D-88F7-828D61CBD5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6559B786-B3D8-409E-9757-03A79C996BEB}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{6559B786-B3D8-409E-9757-03A79C996BEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>BE Services</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Stats</t>
   </si>
   <si>
-    <t>User Info</t>
-  </si>
-  <si>
     <t>Responsável por oferecer as noticias aos utilizadores</t>
   </si>
   <si>
@@ -54,31 +51,67 @@
     <t>Responsável por todas as funcionalidades relacionadas com as carnes</t>
   </si>
   <si>
-    <t>Responsável pela autenticação e configuração da aplicação</t>
-  </si>
-  <si>
-    <t>Uma noticia</t>
-  </si>
-  <si>
-    <t>Estatisticas positivas e negativas</t>
-  </si>
-  <si>
-    <t>Utilizador e definições</t>
-  </si>
-  <si>
-    <t>Supermarket</t>
-  </si>
-  <si>
-    <t>Save</t>
-  </si>
-  <si>
     <t>Product</t>
   </si>
   <si>
-    <t>Carnes, feedback</t>
-  </si>
-  <si>
     <t>Supermercados, Categorias de carnes</t>
+  </si>
+  <si>
+    <t>Market</t>
+  </si>
+  <si>
+    <t>Responsável pelas funcionalidades de mercados/ mercados especificos.</t>
+  </si>
+  <si>
+    <t>Product In Market</t>
+  </si>
+  <si>
+    <t>Responsável por relacionar os produtos com os supermercados</t>
+  </si>
+  <si>
+    <t>Responsável pelas funcionalidades de objetos guardados</t>
+  </si>
+  <si>
+    <t>Produtos, Utilizador</t>
+  </si>
+  <si>
+    <t>Lista de noticia</t>
+  </si>
+  <si>
+    <t>Lista de estatisticas positivas e negativas</t>
+  </si>
+  <si>
+    <t>Responsável pela configuração da aplicação</t>
+  </si>
+  <si>
+    <t>Responsável pela autenticação</t>
+  </si>
+  <si>
+    <t>App Config</t>
+  </si>
+  <si>
+    <t>Definições</t>
+  </si>
+  <si>
+    <t>Utilizador</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Saved</t>
+  </si>
+  <si>
+    <t>Supermercados</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>Carnes</t>
+  </si>
+  <si>
+    <t>Responsável pelo feedback dos utilizadores</t>
   </si>
 </sst>
 </file>
@@ -122,13 +155,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -444,14 +480,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E09D26E6-0304-44BF-80C1-057C64A42590}">
-  <dimension ref="B2:D8"/>
+  <dimension ref="B2:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="5.88671875" customWidth="1"/>
     <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.6640625" bestFit="1" customWidth="1"/>
@@ -469,60 +506,102 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+      <c r="D6" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alterações feitas de modo a ficarem mais em conformidade com o que é pedido
</commit_message>
<xml_diff>
--- a/back-end/Back-end Services.xlsx
+++ b/back-end/Back-end Services.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guicu\Documents\Universidade\Mestrado\2Semestre\Aplicações na web\aw-project\back-end\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\OneDrive\Ambiente de Trabalho\MESTRADO\2 semestre\Aplicações em Web\aw-project\back-end\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05EB8880-0518-412D-88F7-828D61CBD5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECF268F-AFB8-4148-8CA5-6D14B1BF7036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{6559B786-B3D8-409E-9757-03A79C996BEB}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{6559B786-B3D8-409E-9757-03A79C996BEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t>Saved</t>
   </si>
   <si>
-    <t>Supermercados</t>
-  </si>
-  <si>
     <t>Feedback</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>Responsável pelo feedback dos utilizadores</t>
+  </si>
+  <si>
+    <t>Supermercados, Produtos</t>
   </si>
 </sst>
 </file>
@@ -184,9 +184,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -224,7 +224,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -330,7 +330,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -472,7 +472,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -486,15 +486,15 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,7 +505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
@@ -516,7 +516,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -527,7 +527,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -538,7 +538,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
@@ -546,21 +546,21 @@
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
@@ -568,10 +568,10 @@
         <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
@@ -582,7 +582,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
@@ -593,7 +593,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>24</v>
       </c>

</xml_diff>